<commit_message>
Atualizações dados 16/07 20h
</commit_message>
<xml_diff>
--- a/data/standing.xlsx
+++ b/data/standing.xlsx
@@ -694,10 +694,10 @@
         <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
@@ -737,7 +737,7 @@
         <v>1966</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>19</v>
@@ -760,13 +760,13 @@
         <v>1980</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G14" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">

</xml_diff>